<commit_message>
Testing home page Made minor tweaks to weather and news presentation updated sample data minor changes to sever and home renamed news_rotation to home_script added to home_script to make id autosumbit
</commit_message>
<xml_diff>
--- a/samples/employees.xlsx
+++ b/samples/employees.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,126 +470,126 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>69522675</v>
+        <v>76053925</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hux</t>
+          <t>Biggs</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Darklighter</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>hux.unknown@scanner.com</t>
+          <t>biggs.darklighter@scanner.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>+1-555-785-3466</t>
+          <t>+1-555-509-8596</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>/images/69522675.jpg</t>
+          <t>/images/76053925.jpg</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>63116406</v>
+        <v>11551099</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Poe</t>
+          <t>Ackbar</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dameron</t>
+          <t>Admiral</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>poe.dameron@scanner.com</t>
+          <t>ackbar.admiral@scanner.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>+1-555-538-7986</t>
+          <t>+1-555-723-4297</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>/images/63116406.jpg</t>
+          <t>/images/11551099.jpg</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>11597042</v>
+        <v>16913356</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rex</t>
+          <t>Kit</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Fisto</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>rex.unknown@scanner.com</t>
+          <t>kit.fisto@scanner.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>+1-555-630-7423</t>
+          <t>+1-555-859-4387</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>/images/11597042.jpg</t>
+          <t>/images/16913356.jpg</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -599,37 +599,37 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>58677831</v>
+        <v>23877456</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Echo</t>
+          <t>Darth</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Vader</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>echo.unknown@scanner.com</t>
+          <t>darth.vader@scanner.com</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>+1-555-652-3218</t>
+          <t>+1-555-592-2257</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>/images/58677831.jpg</t>
+          <t>/images/23877456.jpg</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -639,47 +639,47 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>19991323</v>
+        <v>96338500</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fives</t>
+          <t>Rex</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Clone</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>fives.unknown@scanner.com</t>
+          <t>rex.clone@scanner.com</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>+1-555-557-3056</t>
+          <t>+1-555-918-5322</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>/images/19991323.jpg</t>
+          <t>/images/96338500.jpg</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -689,37 +689,37 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>25443363</v>
+        <v>58438572</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Echo</t>
+          <t>Figrin</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>D'an</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>echo.unknown@scanner.com</t>
+          <t>figrin.dan@scanner.com</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>+1-555-562-1413</t>
+          <t>+1-555-134-8627</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>/images/25443363.jpg</t>
+          <t>/images/58438572.jpg</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -740,36 +740,36 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>18876994</v>
+        <v>66851394</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mace</t>
+          <t>K2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Windu</t>
+          <t>SO</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>mace.windu@scanner.com</t>
+          <t>k2.so@scanner.com</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>+1-555-263-8348</t>
+          <t>+1-555-163-6151</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>/images/18876994.jpg</t>
+          <t>/images/66851394.jpg</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -779,13 +779,13 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>67914148</v>
+        <v>86262169</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -804,17 +804,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>+1-555-112-8785</t>
+          <t>+1-555-354-6410</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>/images/67914148.jpg</t>
+          <t>/images/86262169.jpg</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -824,42 +824,42 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>16546959</v>
+        <v>27265478</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kylo</t>
+          <t>Tarkin</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ren</t>
+          <t>Wilhuff</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>kylo.ren@scanner.com</t>
+          <t>tarkin.wilhuff@scanner.com</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>+1-555-936-9105</t>
+          <t>+1-555-648-7507</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>/images/16546959.jpg</t>
+          <t>/images/27265478.jpg</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -875,31 +875,31 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>46314080</v>
+        <v>12365101</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cassian</t>
+          <t>Aurra</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Andor</t>
+          <t>Sing</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>cassian.andor@scanner.com</t>
+          <t>aurra.sing@scanner.com</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>+1-555-384-7505</t>
+          <t>+1-555-609-6356</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>/images/46314080.jpg</t>
+          <t>/images/12365101.jpg</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -909,52 +909,52 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>12168691</v>
+        <v>23153615</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cassian</t>
+          <t>Cara</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Andor</t>
+          <t>Dune</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>cassian.andor@scanner.com</t>
+          <t>cara.dune@scanner.com</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>+1-555-587-4031</t>
+          <t>+1-555-984-4985</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>/images/12168691.jpg</t>
+          <t>/images/23153615.jpg</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -965,36 +965,36 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>50563160</v>
+        <v>53912868</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Kylo</t>
+          <t>Phasma</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ren</t>
+          <t>Captain</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>kylo.ren@scanner.com</t>
+          <t>phasma.captain@scanner.com</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>+1-555-910-8241</t>
+          <t>+1-555-647-6231</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>/images/50563160.jpg</t>
+          <t>/images/53912868.jpg</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1010,126 +1010,126 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>93382640</v>
+        <v>82801583</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Chirrut</t>
+          <t>Qi'ra</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Îmwe</t>
+          <t>Crimson</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>chirrut.îmwe@scanner.com</t>
+          <t>qira.crimson@scanner.com</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>+1-555-262-1372</t>
+          <t>+1-555-129-2753</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>/images/93382640.jpg</t>
+          <t>/images/82801583.jpg</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>65637642</v>
+        <v>59335103</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cody</t>
+          <t>Rieekan</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Carlist</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>cody.unknown@scanner.com</t>
+          <t>rieekan.carlist@scanner.com</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>+1-555-388-7300</t>
+          <t>+1-555-611-5432</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>/images/65637642.jpg</t>
+          <t>/images/59335103.jpg</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>69280947</v>
+        <v>22219010</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Enfys</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Fisto</t>
+          <t>Nest</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>kit.fisto@scanner.com</t>
+          <t>enfys.nest@scanner.com</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>+1-555-105-5577</t>
+          <t>+1-555-573-8475</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>/images/69280947.jpg</t>
+          <t>/images/22219010.jpg</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1139,37 +1139,37 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>51296666</v>
+        <v>82624315</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ventress</t>
+          <t>Leia</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Organa</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ventress.unknown@scanner.com</t>
+          <t>leia.organa@scanner.com</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>+1-555-261-3964</t>
+          <t>+1-555-404-8475</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>/images/51296666.jpg</t>
+          <t>/images/82624315.jpg</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1179,52 +1179,52 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>83081968</v>
+        <v>47417325</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Rex</t>
+          <t>Shmi</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Skywalker</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>rex.unknown@scanner.com</t>
+          <t>shmi.skywalker@scanner.com</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>+1-555-977-7079</t>
+          <t>+1-555-841-9777</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>/images/83081968.jpg</t>
+          <t>/images/47417325.jpg</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1235,126 +1235,126 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>88413613</v>
+        <v>63066923</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Chewbacca</t>
+          <t>Han</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Wookiee</t>
+          <t>Solo</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>chewbacca.wookiee@scanner.com</t>
+          <t>han.solo@scanner.com</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>+1-555-858-6577</t>
+          <t>+1-555-796-5542</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>/images/88413613.jpg</t>
+          <t>/images/63066923.jpg</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>79522706</v>
+        <v>67896747</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sabine</t>
+          <t>Barriss</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Wren</t>
+          <t>Offee</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>sabine.wren@scanner.com</t>
+          <t>barriss.offee@scanner.com</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>+1-555-706-4952</t>
+          <t>+1-555-101-3671</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>/images/79522706.jpg</t>
+          <t>/images/67896747.jpg</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>17366290</v>
+        <v>23205174</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Wedge</t>
+          <t>Bossk</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Antilles</t>
+          <t>Trandoshan</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>wedge.antilles@scanner.com</t>
+          <t>bossk.trandoshan@scanner.com</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>+1-555-135-9788</t>
+          <t>+1-555-659-2340</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>/images/17366290.jpg</t>
+          <t>/images/23205174.jpg</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1370,131 +1370,131 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>81392714</v>
+        <v>40596705</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sabine</t>
+          <t>Ozzel</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Wren</t>
+          <t>Kendal</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>sabine.wren@scanner.com</t>
+          <t>ozzel.kendal@scanner.com</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>+1-555-234-9140</t>
+          <t>+1-555-924-5111</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>/images/81392714.jpg</t>
+          <t>/images/40596705.jpg</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>23987737</v>
+        <v>54683398</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Wedge</t>
+          <t>Watto</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Antilles</t>
+          <t>Junklord</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>wedge.antilles@scanner.com</t>
+          <t>watto.junklord@scanner.com</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>+1-555-213-3197</t>
+          <t>+1-555-246-4426</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>/images/23987737.jpg</t>
+          <t>/images/54683398.jpg</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>86388245</v>
+        <v>28559784</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Anakin</t>
+          <t>Poe</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Skywalker</t>
+          <t>Dameron</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>anakin.skywalker@scanner.com</t>
+          <t>poe.dameron@scanner.com</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>+1-555-289-5108</t>
+          <t>+1-555-970-7858</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>/images/86388245.jpg</t>
+          <t>/images/28559784.jpg</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1505,31 +1505,31 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>51681433</v>
+        <v>36737512</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Aurra</t>
+          <t>Baze</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Sing</t>
+          <t>Malbus</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>aurra.sing@scanner.com</t>
+          <t>baze.malbus@scanner.com</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>+1-555-728-4640</t>
+          <t>+1-555-881-2548</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>/images/51681433.jpg</t>
+          <t>/images/36737512.jpg</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1539,42 +1539,42 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>23082833</v>
+        <v>40327575</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bossk</t>
+          <t>Admiral</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Ackbar</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>bossk.unknown@scanner.com</t>
+          <t>admiral.ackbar@scanner.com</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>+1-555-886-6206</t>
+          <t>+1-555-493-7594</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>/images/23082833.jpg</t>
+          <t>/images/40327575.jpg</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1584,42 +1584,42 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>21966219</v>
+        <v>32180005</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Poe</t>
+          <t>Veers</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Dameron</t>
+          <t>Maximilian</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>poe.dameron@scanner.com</t>
+          <t>veers.maximilian@scanner.com</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>+1-555-725-6005</t>
+          <t>+1-555-462-6129</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>/images/21966219.jpg</t>
+          <t>/images/32180005.jpg</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1634,87 +1634,87 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>43114819</v>
+        <v>86368191</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Leia</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Organa</t>
+          <t>Rebo</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>leia.organa@scanner.com</t>
+          <t>max.rebo@scanner.com</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>+1-555-876-9803</t>
+          <t>+1-555-765-4252</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>/images/43114819.jpg</t>
+          <t>/images/86368191.jpg</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>15907223</v>
+        <v>66097761</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Palpatine</t>
+          <t>Jerjerrod</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Sidious</t>
+          <t>Tiaan</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>palpatine.sidious@scanner.com</t>
+          <t>jerjerrod.tiaan@scanner.com</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>+1-555-671-9609</t>
+          <t>+1-555-726-8666</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>/images/15907223.jpg</t>
+          <t>/images/66097761.jpg</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1724,37 +1724,37 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29620721</v>
+        <v>83824399</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Aurra</t>
+          <t>Kylo</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Sing</t>
+          <t>Ren</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>aurra.sing@scanner.com</t>
+          <t>kylo.ren@scanner.com</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>+1-555-865-7590</t>
+          <t>+1-555-715-7524</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>/images/29620721.jpg</t>
+          <t>/images/83824399.jpg</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1769,132 +1769,132 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>10525687</v>
+        <v>80258949</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Yoda</t>
+          <t>Ahsoka</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Tano</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>yoda.unknown@scanner.com</t>
+          <t>ahsoka.tano@scanner.com</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>+1-555-763-2767</t>
+          <t>+1-555-877-7536</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>/images/10525687.jpg</t>
+          <t>/images/80258949.jpg</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>83887054</v>
+        <v>74670650</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Finn</t>
+          <t>Bib</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Fortuna</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>finn.unknown@scanner.com</t>
+          <t>bib.fortuna@scanner.com</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>+1-555-856-3827</t>
+          <t>+1-555-709-8482</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>/images/83887054.jpg</t>
+          <t>/images/74670650.jpg</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>27228538</v>
+        <v>77611549</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Ezra</t>
+          <t>Fives</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Bridger</t>
+          <t>Clone</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ezra.bridger@scanner.com</t>
+          <t>fives.clone@scanner.com</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>+1-555-745-8759</t>
+          <t>+1-555-313-8824</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>/images/27228538.jpg</t>
+          <t>/images/77611549.jpg</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1910,41 +1910,41 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>80574213</v>
+        <v>97136304</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Din</t>
+          <t>Maz</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Djarin</t>
+          <t>Kanata</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>din.djarin@scanner.com</t>
+          <t>maz.kanata@scanner.com</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>+1-555-908-7700</t>
+          <t>+1-555-458-8364</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>/images/80574213.jpg</t>
+          <t>/images/97136304.jpg</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -1955,36 +1955,36 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>25405500</v>
+        <v>51215523</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Yoda</t>
+          <t>Mace</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Windu</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>yoda.unknown@scanner.com</t>
+          <t>mace.windu@scanner.com</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>+1-555-865-8657</t>
+          <t>+1-555-689-7175</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>/images/25405500.jpg</t>
+          <t>/images/51215523.jpg</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1994,127 +1994,127 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>46307070</v>
+        <v>56465093</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Lando</t>
+          <t>Chewbacca</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Calrissian</t>
+          <t>Wookiee</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>lando.calrissian@scanner.com</t>
+          <t>chewbacca.wookiee@scanner.com</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>+1-555-535-8087</t>
+          <t>+1-555-480-5804</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>/images/46307070.jpg</t>
+          <t>/images/56465093.jpg</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>39447869</v>
+        <v>57295327</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Anakin</t>
+          <t>Unkar</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Skywalker</t>
+          <t>Plutt</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>anakin.skywalker@scanner.com</t>
+          <t>unkar.plutt@scanner.com</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>+1-555-482-8125</t>
+          <t>+1-555-937-5097</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>/images/39447869.jpg</t>
+          <t>/images/57295327.jpg</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>78311480</v>
+        <v>37230127</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cody</t>
+          <t>Dexter</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Jetster</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>cody.unknown@scanner.com</t>
+          <t>dexter.jetster@scanner.com</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>+1-555-852-9688</t>
+          <t>+1-555-946-2305</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>/images/78311480.jpg</t>
+          <t>/images/37230127.jpg</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2129,82 +2129,82 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>44554577</v>
+        <v>64889551</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Lando</t>
+          <t>Cliegg</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Calrissian</t>
+          <t>Lars</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>lando.calrissian@scanner.com</t>
+          <t>cliegg.lars@scanner.com</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>+1-555-723-9619</t>
+          <t>+1-555-836-6422</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>/images/44554577.jpg</t>
+          <t>/images/64889551.jpg</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>82213638</v>
+        <v>37983314</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Chewbacca</t>
+          <t>Cassian</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Wookiee</t>
+          <t>Andor</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>chewbacca.wookiee@scanner.com</t>
+          <t>cassian.andor@scanner.com</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>+1-555-217-3453</t>
+          <t>+1-555-618-3838</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>/images/82213638.jpg</t>
+          <t>/images/37983314.jpg</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2214,47 +2214,47 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>86945173</v>
+        <v>56401407</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Mace</t>
+          <t>Dodonna</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Windu</t>
+          <t>Jan</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>mace.windu@scanner.com</t>
+          <t>dodonna.jan@scanner.com</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>+1-555-925-9281</t>
+          <t>+1-555-573-7271</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>/images/86945173.jpg</t>
+          <t>/images/56401407.jpg</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2270,126 +2270,126 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>14117166</v>
+        <v>21391142</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Grogu</t>
+          <t>DJ</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Blunt</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>grogu.unknown@scanner.com</t>
+          <t>dj.blunt@scanner.com</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>+1-555-831-6626</t>
+          <t>+1-555-440-4704</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>/images/14117166.jpg</t>
+          <t>/images/21391142.jpg</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>28945036</v>
+        <v>55737291</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Barriss</t>
+          <t>Qui-Gon</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Offee</t>
+          <t>Jinn</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>barriss.offee@scanner.com</t>
+          <t>qui-gon.jinn@scanner.com</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>+1-555-741-1703</t>
+          <t>+1-555-569-7720</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>/images/28945036.jpg</t>
+          <t>/images/55737291.jpg</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>61523647</v>
+        <v>35728086</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Sabine</t>
+          <t>Aayla</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Wren</t>
+          <t>Secura</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>sabine.wren@scanner.com</t>
+          <t>aayla.secura@scanner.com</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>+1-555-192-1643</t>
+          <t>+1-555-686-7374</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>/images/61523647.jpg</t>
+          <t>/images/35728086.jpg</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2399,172 +2399,172 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>82248201</v>
+        <v>92715041</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Kylo</t>
+          <t>Ventress</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ren</t>
+          <t>Asajj</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>kylo.ren@scanner.com</t>
+          <t>ventress.asajj@scanner.com</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>+1-555-953-2483</t>
+          <t>+1-555-576-6347</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>/images/82248201.jpg</t>
+          <t>/images/92715041.jpg</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>51717476</v>
+        <v>92363416</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Han</t>
+          <t>Hondo</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Solo</t>
+          <t>Ohnaka</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>han.solo@scanner.com</t>
+          <t>hondo.ohnaka@scanner.com</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>+1-555-537-3045</t>
+          <t>+1-555-460-9081</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>/images/51717476.jpg</t>
+          <t>/images/92363416.jpg</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>42133906</v>
+        <v>42269120</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Baze</t>
+          <t>Din</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Malbus</t>
+          <t>Djarin</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>baze.malbus@scanner.com</t>
+          <t>din.djarin@scanner.com</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>+1-555-196-8591</t>
+          <t>+1-555-872-2045</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>/images/42133906.jpg</t>
+          <t>/images/42269120.jpg</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>22221253</v>
+        <v>65001426</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Hux</t>
+          <t>Greedo</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Rodian</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>hux.unknown@scanner.com</t>
+          <t>greedo.rodian@scanner.com</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>+1-555-705-6691</t>
+          <t>+1-555-109-4785</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>/images/22221253.jpg</t>
+          <t>/images/65001426.jpg</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2574,92 +2574,92 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>17342130</v>
+        <v>81685045</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Luke</t>
+          <t>Beckett</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Skywalker</t>
+          <t>Tobias</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>luke.skywalker@scanner.com</t>
+          <t>beckett.tobias@scanner.com</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>+1-555-823-3012</t>
+          <t>+1-555-201-4707</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>/images/17342130.jpg</t>
+          <t>/images/81685045.jpg</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>85558584</v>
+        <v>57693970</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Din</t>
+          <t>Saw</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Djarin</t>
+          <t>Gerrera</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>din.djarin@scanner.com</t>
+          <t>saw.gerrera@scanner.com</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>+1-555-228-8047</t>
+          <t>+1-555-601-9086</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>/images/85558584.jpg</t>
+          <t>/images/57693970.jpg</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2669,82 +2669,82 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>55732850</v>
+        <v>70641528</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Boba</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Fisto</t>
+          <t>Fett</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>kit.fisto@scanner.com</t>
+          <t>boba.fett@scanner.com</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>+1-555-218-7777</t>
+          <t>+1-555-118-7381</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>/images/55732850.jpg</t>
+          <t>/images/70641528.jpg</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>23874001</v>
+        <v>77568598</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Anakin</t>
+          <t>Hux</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Skywalker</t>
+          <t>Armitage</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>anakin.skywalker@scanner.com</t>
+          <t>hux.armitage@scanner.com</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>+1-555-193-2373</t>
+          <t>+1-555-655-2048</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>/images/23874001.jpg</t>
+          <t>/images/77568598.jpg</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2754,92 +2754,92 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>24301995</v>
+        <v>90118025</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Fives</t>
+          <t>Cad</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Bane</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>fives.unknown@scanner.com</t>
+          <t>cad.bane@scanner.com</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>+1-555-599-4203</t>
+          <t>+1-555-485-1569</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>/images/24301995.jpg</t>
+          <t>/images/90118025.jpg</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>56398042</v>
+        <v>96776710</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Han</t>
+          <t>Sy</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Solo</t>
+          <t>Snootles</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>han.solo@scanner.com</t>
+          <t>sy.snootles@scanner.com</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>+1-555-664-6741</t>
+          <t>+1-555-238-6545</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>/images/56398042.jpg</t>
+          <t>/images/96776710.jpg</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2855,36 +2855,36 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>69073491</v>
+        <v>19896102</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Qui-Gon</t>
+          <t>Sabine</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Jinn</t>
+          <t>Wren</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>qui-gon.jinn@scanner.com</t>
+          <t>sabine.wren@scanner.com</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>+1-555-990-9622</t>
+          <t>+1-555-195-7649</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>/images/69073491.jpg</t>
+          <t>/images/19896102.jpg</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2894,132 +2894,132 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>95798266</v>
+        <v>81588124</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Admiral</t>
+          <t>Lando</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Ackbar</t>
+          <t>Calrissian</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>admiral.ackbar@scanner.com</t>
+          <t>lando.calrissian@scanner.com</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>+1-555-151-3777</t>
+          <t>+1-555-329-7904</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>/images/95798266.jpg</t>
+          <t>/images/81588124.jpg</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Project Lead</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>41933058</v>
+        <v>89400093</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Piett</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Mothma</t>
+          <t>Firmus</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>mon.mothma@scanner.com</t>
+          <t>piett.firmus@scanner.com</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>+1-555-263-7956</t>
+          <t>+1-555-605-9291</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>/images/41933058.jpg</t>
+          <t>/images/89400093.jpg</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>82539808</v>
+        <v>99134812</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Rey</t>
+          <t>Bail</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Palpatine</t>
+          <t>Organa</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>rey.palpatine@scanner.com</t>
+          <t>bail.organa@scanner.com</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>+1-555-520-8513</t>
+          <t>+1-555-903-1792</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>/images/82539808.jpg</t>
+          <t>/images/99134812.jpg</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3029,87 +3029,87 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>73669954</v>
+        <v>34056567</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Lando</t>
+          <t>Rose</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Calrissian</t>
+          <t>Tico</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>lando.calrissian@scanner.com</t>
+          <t>rose.tico@scanner.com</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>+1-555-569-6056</t>
+          <t>+1-555-797-1908</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>/images/73669954.jpg</t>
+          <t>/images/34056567.jpg</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>60420528</v>
+        <v>43712755</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Kit</t>
+          <t>Shaak</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Fisto</t>
+          <t>Ti</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>kit.fisto@scanner.com</t>
+          <t>shaak.ti@scanner.com</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>+1-555-292-5261</t>
+          <t>+1-555-586-1310</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>/images/60420528.jpg</t>
+          <t>/images/43712755.jpg</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -3119,82 +3119,82 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>84572277</v>
+        <v>75858902</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Kylo</t>
+          <t>Droopy</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Ren</t>
+          <t>McCool</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>kylo.ren@scanner.com</t>
+          <t>droopy.mccool@scanner.com</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>+1-555-144-6946</t>
+          <t>+1-555-353-2028</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>/images/84572277.jpg</t>
+          <t>/images/75858902.jpg</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>69689621</v>
+        <v>18617297</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Poe</t>
+          <t>Ezra</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Dameron</t>
+          <t>Bridger</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>poe.dameron@scanner.com</t>
+          <t>ezra.bridger@scanner.com</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>+1-555-918-4948</t>
+          <t>+1-555-791-6258</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>/images/69689621.jpg</t>
+          <t>/images/18617297.jpg</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -3204,42 +3204,42 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Security &amp; Strategy</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>57533195</v>
+        <v>94986959</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Hux</t>
+          <t>Cody</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Clone</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>hux.unknown@scanner.com</t>
+          <t>cody.clone@scanner.com</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>+1-555-505-1696</t>
+          <t>+1-555-268-3361</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>/images/57533195.jpg</t>
+          <t>/images/94986959.jpg</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -3249,47 +3249,47 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>72830634</v>
+        <v>68543144</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Bossk</t>
+          <t>Anakin</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Skywalker</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>bossk.unknown@scanner.com</t>
+          <t>anakin.skywalker@scanner.com</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>+1-555-407-8147</t>
+          <t>+1-555-673-8354</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>/images/72830634.jpg</t>
+          <t>/images/68543144.jpg</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -3299,82 +3299,82 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>87438453</v>
+        <v>13053923</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Cassian</t>
+          <t>Bo-Katan</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Andor</t>
+          <t>Kryze</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>cassian.andor@scanner.com</t>
+          <t>bo-katan.kryze@scanner.com</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>+1-555-842-8992</t>
+          <t>+1-555-281-4436</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>/images/87438453.jpg</t>
+          <t>/images/13053923.jpg</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>12986841</v>
+        <v>59694871</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Wedge</t>
+          <t>Chirrut</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Antilles</t>
+          <t>Îmwe</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>wedge.antilles@scanner.com</t>
+          <t>chirrut.îmwe@scanner.com</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>+1-555-304-5433</t>
+          <t>+1-555-839-6088</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>/images/12986841.jpg</t>
+          <t>/images/59694871.jpg</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -3384,132 +3384,132 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>49484902</v>
+        <v>24724933</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Wedge</t>
+          <t>Hera</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Antilles</t>
+          <t>Syndulla</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>wedge.antilles@scanner.com</t>
+          <t>hera.syndulla@scanner.com</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>+1-555-813-6286</t>
+          <t>+1-555-480-4904</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>/images/49484902.jpg</t>
+          <t>/images/24724933.jpg</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>89560833</v>
+        <v>57987062</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Padmé</t>
+          <t>Thrawn</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Amidala</t>
+          <t>Mitthraw</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>padmé.amidala@scanner.com</t>
+          <t>thrawn.mitthraw@scanner.com</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>+1-555-528-8749</t>
+          <t>+1-555-386-3628</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>/images/89560833.jpg</t>
+          <t>/images/57987062.jpg</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>91952924</v>
+        <v>58222720</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Phasma</t>
+          <t>Finn</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Tico</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>phasma.unknown@scanner.com</t>
+          <t>finn.tico@scanner.com</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>+1-555-143-2374</t>
+          <t>+1-555-627-1700</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>/images/91952924.jpg</t>
+          <t>/images/58222720.jpg</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -3519,52 +3519,52 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>32730745</v>
+        <v>50787242</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Cad</t>
+          <t>Obi-Wan</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Bane</t>
+          <t>Kenobi</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>cad.bane@scanner.com</t>
+          <t>obi-wan.kenobi@scanner.com</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>+1-555-734-7654</t>
+          <t>+1-555-102-1539</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>/images/32730745.jpg</t>
+          <t>/images/50787242.jpg</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -3575,41 +3575,41 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>14768621</v>
+        <v>63251534</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Hera</t>
+          <t>Sidon</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Syndulla</t>
+          <t>Ithano</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>hera.syndulla@scanner.com</t>
+          <t>sidon.ithano@scanner.com</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>+1-555-791-1304</t>
+          <t>+1-555-703-1458</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>/images/14768621.jpg</t>
+          <t>/images/63251534.jpg</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -3620,76 +3620,76 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>65364136</v>
+        <v>81122398</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>IG-88</t>
+          <t>Elan</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Sleazebaggano</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>ig-88.unknown@scanner.com</t>
+          <t>elan.sleazebaggano@scanner.com</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>+1-555-955-4290</t>
+          <t>+1-555-874-8458</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>/images/65364136.jpg</t>
+          <t>/images/81122398.jpg</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>58949404</v>
+        <v>56676067</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Obi-Wan</t>
+          <t>Padmé</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Kenobi</t>
+          <t>Amidala</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>obi-wan.kenobi@scanner.com</t>
+          <t>padmé.amidala@scanner.com</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>+1-555-767-7235</t>
+          <t>+1-555-207-5077</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>/images/58949404.jpg</t>
+          <t>/images/56676067.jpg</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -3704,37 +3704,37 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>64883113</v>
+        <v>18257529</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Qui-Gon</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Jinn</t>
+          <t>Mothma</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>qui-gon.jinn@scanner.com</t>
+          <t>mon.mothma@scanner.com</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>+1-555-500-5812</t>
+          <t>+1-555-245-1306</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>/images/64883113.jpg</t>
+          <t>/images/18257529.jpg</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -3749,37 +3749,37 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Droid Services</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>58636842</v>
+        <v>95899622</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Cad</t>
+          <t>Rey</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Bane</t>
+          <t>Palpatine</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>cad.bane@scanner.com</t>
+          <t>rey.palpatine@scanner.com</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>+1-555-797-4654</t>
+          <t>+1-555-318-4006</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>/images/58636842.jpg</t>
+          <t>/images/95899622.jpg</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -3789,187 +3789,187 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>84592281</v>
+        <v>83606015</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Bo-Katan</t>
+          <t>Jyn</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Kryze</t>
+          <t>Erso</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>bo-katan.kryze@scanner.com</t>
+          <t>jyn.erso@scanner.com</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>+1-555-484-6455</t>
+          <t>+1-555-329-7474</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>/images/84592281.jpg</t>
+          <t>/images/83606015.jpg</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>Droid Services</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>80061301</v>
+        <v>76116542</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Hux</t>
+          <t>Zam</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Wesell</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>hux.unknown@scanner.com</t>
+          <t>zam.wesell@scanner.com</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>+1-555-428-5978</t>
+          <t>+1-555-481-5893</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>/images/80061301.jpg</t>
+          <t>/images/76116542.jpg</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Senior Officer</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>Rebel Relations</t>
+          <t>Galactic Operations</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>20793921</v>
+        <v>29198138</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Leia</t>
+          <t>Val</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Organa</t>
+          <t>Beckett</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>leia.organa@scanner.com</t>
+          <t>val.beckett@scanner.com</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>+1-555-879-5490</t>
+          <t>+1-555-439-2568</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>/images/20793921.jpg</t>
+          <t>/images/29198138.jpg</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Rebel Relations</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>43654476</v>
+        <v>51731925</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Chirrut</t>
+          <t>Holdo</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Îmwe</t>
+          <t>Amilyn</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>chirrut.îmwe@scanner.com</t>
+          <t>holdo.amilyn@scanner.com</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>+1-555-650-3864</t>
+          <t>+1-555-598-1050</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>/images/43654476.jpg</t>
+          <t>/images/51731925.jpg</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Support Specialist</t>
+          <t>Associate</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Coordinator</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -3980,31 +3980,31 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>97627493</v>
+        <v>54263237</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Cara</t>
+          <t>Sebulba</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Dune</t>
+          <t>Podracer</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>cara.dune@scanner.com</t>
+          <t>sebulba.podracer@scanner.com</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>+1-555-391-4584</t>
+          <t>+1-555-167-7567</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>/images/97627493.jpg</t>
+          <t>/images/54263237.jpg</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -4025,31 +4025,31 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>64954925</v>
+        <v>77869293</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Thrawn</t>
+          <t>Lor</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>San</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>thrawn.unknown@scanner.com</t>
+          <t>lor.san@scanner.com</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>+1-555-934-2273</t>
+          <t>+1-555-294-2818</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>/images/64954925.jpg</t>
+          <t>/images/77869293.jpg</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -4059,7 +4059,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Manager</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -4070,81 +4070,81 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>82537373</v>
+        <v>50495184</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Grogu</t>
+          <t>Palpatine</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Sidious</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>grogu.unknown@scanner.com</t>
+          <t>palpatine.sidious@scanner.com</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>+1-555-823-8502</t>
+          <t>+1-555-111-3154</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>/images/82537373.jpg</t>
+          <t>/images/50495184.jpg</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>Galactic Operations</t>
+          <t>Security &amp; Strategy</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>76600519</v>
+        <v>47834449</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Baze</t>
+          <t>Needa</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Malbus</t>
+          <t>Lorth</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>baze.malbus@scanner.com</t>
+          <t>needa.lorth@scanner.com</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>+1-555-767-6890</t>
+          <t>+1-555-404-2303</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>/images/76600519.jpg</t>
+          <t>/images/47834449.jpg</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Associate</t>
+          <t>Senior Officer</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -4160,41 +4160,41 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>91519977</v>
+        <v>25587577</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Han</t>
+          <t>Echo</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Solo</t>
+          <t>Clone</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>han.solo@scanner.com</t>
+          <t>echo.clone@scanner.com</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>+1-555-454-3067</t>
+          <t>+1-555-456-8582</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>/images/91519977.jpg</t>
+          <t>/images/25587577.jpg</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Project Lead</t>
+          <t>Support Specialist</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Manager</t>
+          <t>Technician</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -4205,31 +4205,31 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>47705171</v>
+        <v>64365795</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Echo</t>
+          <t>Wedge</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Antilles</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>echo.unknown@scanner.com</t>
+          <t>wedge.antilles@scanner.com</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>+1-555-391-6924</t>
+          <t>+1-555-293-5760</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>/images/47705171.jpg</t>
+          <t>/images/64365795.jpg</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -4239,732 +4239,12 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Coordinator</t>
+          <t>Analyst</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
           <t>Security &amp; Strategy</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>74874792</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Yoda</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>yoda.unknown@scanner.com</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>+1-555-583-3888</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>/images/74874792.jpg</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Associate</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Technician</t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>Rebel Relations</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>45177456</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Admiral</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Ackbar</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>admiral.ackbar@scanner.com</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>+1-555-758-7684</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>/images/45177456.jpg</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Support Specialist</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Technician</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>Security &amp; Strategy</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>54359600</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>K2</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>k2.so@scanner.com</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>+1-555-788-9003</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>/images/54359600.jpg</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Senior Officer</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Manager</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>Droid Services</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>29645196</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Aurra</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Sing</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>aurra.sing@scanner.com</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>+1-555-540-7568</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>/images/29645196.jpg</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Project Lead</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Manager</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>Security &amp; Strategy</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>38285369</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Admiral</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Ackbar</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>admiral.ackbar@scanner.com</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>+1-555-421-7485</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>/images/38285369.jpg</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Senior Officer</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Technician</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>Rebel Relations</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>39920951</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Finn</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>finn.unknown@scanner.com</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>+1-555-542-2961</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>/images/39920951.jpg</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Associate</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Technician</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>Security &amp; Strategy</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>82523788</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Cad</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Bane</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>cad.bane@scanner.com</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>+1-555-895-3444</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>/images/82523788.jpg</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Support Specialist</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Manager</t>
-        </is>
-      </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>Galactic Operations</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>76031763</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Ventress</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>ventress.unknown@scanner.com</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>+1-555-501-9999</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>/images/76031763.jpg</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>Project Lead</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>Analyst</t>
-        </is>
-      </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>Droid Services</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>56425652</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>K2</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>SO</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>k2.so@scanner.com</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>+1-555-806-8078</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>/images/56425652.jpg</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>Senior Officer</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Technician</t>
-        </is>
-      </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>Droid Services</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>67023662</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Mace</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Windu</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>mace.windu@scanner.com</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>+1-555-420-3713</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>/images/67023662.jpg</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>Associate</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>Coordinator</t>
-        </is>
-      </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>Security &amp; Strategy</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>36807107</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Cody</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>cody.unknown@scanner.com</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>+1-555-228-1868</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>/images/36807107.jpg</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Senior Officer</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Technician</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>Droid Services</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>88196117</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Mothma</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>mon.mothma@scanner.com</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>+1-555-370-8161</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>/images/88196117.jpg</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>Associate</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>Manager</t>
-        </is>
-      </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>Droid Services</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>68569011</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Ezra</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Bridger</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>ezra.bridger@scanner.com</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>+1-555-650-3477</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>/images/68569011.jpg</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>Associate</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>Manager</t>
-        </is>
-      </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>Galactic Operations</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>34031280</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Bossk</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>bossk.unknown@scanner.com</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>+1-555-734-8321</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>/images/34031280.jpg</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>Senior Officer</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>Coordinator</t>
-        </is>
-      </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>Rebel Relations</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>57539479</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Thrawn</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>thrawn.unknown@scanner.com</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>+1-555-899-5036</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>/images/57539479.jpg</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>Associate</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>Analyst</t>
-        </is>
-      </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>Droid Services</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>24865293</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Wedge</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Antilles</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>wedge.antilles@scanner.com</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>+1-555-747-6173</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>/images/24865293.jpg</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>Support Specialist</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>Analyst</t>
-        </is>
-      </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>Galactic Operations</t>
         </is>
       </c>
     </row>

</xml_diff>